<commit_message>
adjustments and fix file validation
</commit_message>
<xml_diff>
--- a/Summer_23/Coding_Assignments/Code4/Output_1001669855.xlsx
+++ b/Summer_23/Coding_Assignments/Code4/Output_1001669855.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/donna_french_uta_edu/Documents/UTA/Coding Assignments/CSE3318 Summer 2023/Coding Assignment 4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_Code\CSE3318\cse3318\Summer_23\Coding_Assignments\Code4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="8_{85AF264F-B6E5-4709-A96A-2CD95392FF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57013203-358B-4BE8-A16D-17F2A9F21E82}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AB194B-22E3-4578-8B2E-A0F992D06481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4A00EAFC-8136-4C01-985A-E9A0D427D15A}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4A00EAFC-8136-4C01-985A-E9A0D427D15A}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -662,15 +662,15 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="11.28515625" customWidth="1"/>
   </cols>
@@ -717,78 +717,162 @@
       <c r="A3" s="9">
         <v>1024</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="3">
+        <v>65</v>
+      </c>
+      <c r="C3" s="3">
+        <v>77</v>
+      </c>
+      <c r="D3" s="3">
+        <v>68</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>10000</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="3">
+        <v>845</v>
+      </c>
+      <c r="C4" s="3">
+        <v>977</v>
+      </c>
+      <c r="D4" s="3">
+        <v>863</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>50000</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="3">
+        <v>4913</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5616</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4771</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10000</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>100000</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="3">
+        <v>10518</v>
+      </c>
+      <c r="C6" s="3">
+        <v>13441</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10412</v>
+      </c>
+      <c r="E6" s="3">
+        <v>16666</v>
+      </c>
+      <c r="F6" s="3">
+        <v>16666</v>
+      </c>
+      <c r="G6" s="3">
+        <v>16666</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>500000</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="3">
+        <v>59430</v>
+      </c>
+      <c r="C7" s="3">
+        <v>76621</v>
+      </c>
+      <c r="D7" s="3">
+        <v>57206</v>
+      </c>
+      <c r="E7" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>106666</v>
+      </c>
+      <c r="G7" s="3">
+        <v>100000</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1000000</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" s="3">
+        <v>117253</v>
+      </c>
+      <c r="C8" s="3">
+        <v>141745</v>
+      </c>
+      <c r="D8" s="3">
+        <v>123255</v>
+      </c>
+      <c r="E8" s="3">
+        <v>203333</v>
+      </c>
+      <c r="F8" s="3">
+        <v>206666</v>
+      </c>
+      <c r="G8" s="3">
+        <v>213333</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>2000000</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="3">
+        <v>248858</v>
+      </c>
+      <c r="C9" s="3">
+        <v>299248</v>
+      </c>
+      <c r="D9" s="3">
+        <v>255117</v>
+      </c>
+      <c r="E9" s="3">
+        <v>420000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>433333</v>
+      </c>
+      <c r="G9" s="3">
+        <v>440000</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -844,46 +928,106 @@
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B14">
+        <v>9551</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10086</v>
+      </c>
+      <c r="D14" s="3">
+        <v>372001</v>
+      </c>
+      <c r="E14" s="3">
+        <v>16902472</v>
+      </c>
+      <c r="F14" s="3">
+        <v>17981814</v>
+      </c>
+      <c r="G14" s="3">
+        <v>16000</v>
+      </c>
+      <c r="H14" s="3">
+        <v>16000</v>
+      </c>
+      <c r="I14" s="3">
+        <v>556000</v>
+      </c>
+      <c r="J14" s="3">
+        <v>24978000</v>
+      </c>
+      <c r="K14" s="3">
+        <v>26728000</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="B15" s="7">
+        <v>11833</v>
+      </c>
+      <c r="C15" s="3">
+        <v>11735</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12088</v>
+      </c>
+      <c r="E15" s="3">
+        <v>6375</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4799</v>
+      </c>
+      <c r="G15" s="3">
+        <v>18000</v>
+      </c>
+      <c r="H15" s="3">
+        <v>18000</v>
+      </c>
+      <c r="I15" s="3">
+        <v>18000</v>
+      </c>
+      <c r="J15" s="3">
+        <v>10000</v>
+      </c>
+      <c r="K15" s="3">
+        <v>6000</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="7"/>
+      <c r="B16" s="7">
+        <v>9378</v>
+      </c>
+      <c r="C16" s="3">
+        <v>9867</v>
+      </c>
+      <c r="D16" s="3">
+        <v>359956</v>
+      </c>
+      <c r="E16" s="3">
+        <v>16062110</v>
+      </c>
+      <c r="F16" s="7">
+        <v>17782280</v>
+      </c>
+      <c r="G16" s="3">
+        <v>18000</v>
+      </c>
+      <c r="H16" s="3">
+        <v>20000</v>
+      </c>
+      <c r="I16" s="3">
+        <v>16000</v>
+      </c>
+      <c r="J16" s="3">
+        <v>14000</v>
+      </c>
+      <c r="K16" s="7">
+        <v>10000</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1230,12 +1374,54 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TeamsChannelId xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Math_Settings xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Owner xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <AppVersion xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Invited_Teachers xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <NotebookType xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <FolderType xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Teachers xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <LMS_Mappings xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Invited_Students xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <CultureName xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Distribution_Groups xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+    <Templates xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1644,60 +1830,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TeamsChannelId xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Math_Settings xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Owner xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <AppVersion xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Invited_Teachers xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <NotebookType xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <FolderType xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Teachers xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <LMS_Mappings xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Invited_Students xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <CultureName xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Distribution_Groups xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-    <Templates xmlns="edc47199-8429-4a30-a8c5-19487a2cfb84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2680113-FCEE-4B54-AA0E-217FBB37140B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61C8FF13-9F74-4FB9-A71F-5902366276EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7c488e8a-7c9d-4a25-ac1a-3919c0dde376"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="edc47199-8429-4a30-a8c5-19487a2cfb84"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1722,18 +1875,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61C8FF13-9F74-4FB9-A71F-5902366276EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2680113-FCEE-4B54-AA0E-217FBB37140B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7c488e8a-7c9d-4a25-ac1a-3919c0dde376"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="edc47199-8429-4a30-a8c5-19487a2cfb84"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
working some more on Code
</commit_message>
<xml_diff>
--- a/Summer_23/Coding_Assignments/Code4/Output_1001669855.xlsx
+++ b/Summer_23/Coding_Assignments/Code4/Output_1001669855.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_Code\CSE3318\cse3318\Summer_23\Coding_Assignments\Code4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AB194B-22E3-4578-8B2E-A0F992D06481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D2CAA-E69F-48C1-A189-620AB218D54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4A00EAFC-8136-4C01-985A-E9A0D427D15A}"/>
+    <workbookView xWindow="-24120" yWindow="3600" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{4A00EAFC-8136-4C01-985A-E9A0D427D15A}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Put your paragraph from Step 10 in this box - just start typing in this box.
-</t>
   </si>
   <si>
     <t>QSR</t>
@@ -89,6 +85,14 @@
   </si>
   <si>
     <t>PC tics - 100,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.) That while all the sort variations are similar with the original data being totally randomized, the right pivot shows to be slightly faster than the other variations, however when the data is partially sorted it suffers jurasitically.                                                                                                                                                                 2.) Yes, as while it doesn't help too much in a randomize data, but when its semi or completely ordered it helps a lot as the time is cut down a lot.
+3.) With randomized data it has similar times to merge sort, however if the data is sorted then the time complexity looks more Insertion sort in the worst case. 
+4.) It depends on the data and if its ordered or not but if its randomized data it does do very well and can be better than merge sort with bigger volumes of data since it does not create additional arrays.
+5.) The quick sort speed depends on the position of the pivot, as with a far right pivot and an ordered dataset has a terrible time complexity, but the others have better time complexity the more sorted they are. 
+6.) Based on the data I would recommend a middle pivot as it had the best results even with a sorted data set.
+</t>
   </si>
 </sst>
 </file>
@@ -360,6 +364,2376 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>n</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> and PC Tics</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>QSR</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>816</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4830</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10331</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56781</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117263</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>245628</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE8F-4FF2-85A1-89E57A36167D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>QSM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71347</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>297518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CE8F-4FF2-85A1-89E57A36167D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>QSRND</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$D$3:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5843</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12317</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69490</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144769</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301466</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CE8F-4FF2-85A1-89E57A36167D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2067315440"/>
+        <c:axId val="2067320720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2067315440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2067320720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2067320720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2067315440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>n</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> and Omega Tics</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>QSR</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>203333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>420000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1EA1-4011-A585-3ACF2DD08249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>QSM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>206666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>433333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1EA1-4011-A585-3ACF2DD08249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>QSRND</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>213333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>440000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1EA1-4011-A585-3ACF2DD08249}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2067315440"/>
+        <c:axId val="2067320720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2067315440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2067320720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2067320720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2067315440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F82AA513-50F6-46AA-1168-60073CDBD779}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{764178E0-8D62-4319-A893-5CEBF93104CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,12 +3031,298 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13FA7EA-335B-484F-A557-606D409DE0A3}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +3338,7 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="14"/>
@@ -695,22 +3355,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -718,13 +3378,13 @@
         <v>1024</v>
       </c>
       <c r="B3" s="3">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -741,13 +3401,13 @@
         <v>10000</v>
       </c>
       <c r="B4" s="3">
-        <v>845</v>
+        <v>816</v>
       </c>
       <c r="C4" s="3">
-        <v>977</v>
+        <v>1005</v>
       </c>
       <c r="D4" s="3">
-        <v>863</v>
+        <v>1044</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -764,13 +3424,13 @@
         <v>50000</v>
       </c>
       <c r="B5" s="3">
-        <v>4913</v>
+        <v>4830</v>
       </c>
       <c r="C5" s="3">
-        <v>5616</v>
+        <v>5916</v>
       </c>
       <c r="D5" s="3">
-        <v>4771</v>
+        <v>5843</v>
       </c>
       <c r="E5" s="3">
         <v>10000</v>
@@ -787,13 +3447,13 @@
         <v>100000</v>
       </c>
       <c r="B6" s="3">
-        <v>10518</v>
+        <v>10331</v>
       </c>
       <c r="C6" s="3">
-        <v>13441</v>
+        <v>12154</v>
       </c>
       <c r="D6" s="3">
-        <v>10412</v>
+        <v>12317</v>
       </c>
       <c r="E6" s="3">
         <v>16666</v>
@@ -810,13 +3470,13 @@
         <v>500000</v>
       </c>
       <c r="B7" s="3">
-        <v>59430</v>
+        <v>56781</v>
       </c>
       <c r="C7" s="3">
-        <v>76621</v>
+        <v>71347</v>
       </c>
       <c r="D7" s="3">
-        <v>57206</v>
+        <v>69490</v>
       </c>
       <c r="E7" s="3">
         <v>100000</v>
@@ -833,13 +3493,13 @@
         <v>1000000</v>
       </c>
       <c r="B8" s="3">
-        <v>117253</v>
+        <v>117263</v>
       </c>
       <c r="C8" s="3">
-        <v>141745</v>
+        <v>142898</v>
       </c>
       <c r="D8" s="3">
-        <v>123255</v>
+        <v>144769</v>
       </c>
       <c r="E8" s="3">
         <v>203333</v>
@@ -856,13 +3516,13 @@
         <v>2000000</v>
       </c>
       <c r="B9" s="3">
-        <v>248858</v>
+        <v>245628</v>
       </c>
       <c r="C9" s="3">
-        <v>299248</v>
+        <v>297518</v>
       </c>
       <c r="D9" s="3">
-        <v>255117</v>
+        <v>301466</v>
       </c>
       <c r="E9" s="3">
         <v>420000</v>
@@ -877,14 +3537,14 @@
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -894,54 +3554,54 @@
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="F13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="K13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>9551</v>
+        <v>9222</v>
       </c>
       <c r="C14" s="3">
-        <v>10086</v>
+        <v>10181</v>
       </c>
       <c r="D14" s="3">
-        <v>372001</v>
+        <v>355522</v>
       </c>
       <c r="E14" s="3">
-        <v>16902472</v>
+        <v>16116284</v>
       </c>
       <c r="F14" s="3">
-        <v>17981814</v>
+        <v>17312205</v>
       </c>
       <c r="G14" s="3">
         <v>16000</v>
@@ -961,22 +3621,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="7">
-        <v>11833</v>
+        <v>12013</v>
       </c>
       <c r="C15" s="3">
-        <v>11735</v>
+        <v>11993</v>
       </c>
       <c r="D15" s="3">
-        <v>12088</v>
+        <v>12089</v>
       </c>
       <c r="E15" s="3">
-        <v>6375</v>
+        <v>6452</v>
       </c>
       <c r="F15" s="7">
-        <v>4799</v>
+        <v>4778</v>
       </c>
       <c r="G15" s="3">
         <v>18000</v>
@@ -996,22 +3656,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="7">
-        <v>9378</v>
+        <v>12512</v>
       </c>
       <c r="C16" s="3">
-        <v>9867</v>
+        <v>11932</v>
       </c>
       <c r="D16" s="3">
-        <v>359956</v>
+        <v>10522</v>
       </c>
       <c r="E16" s="3">
-        <v>16062110</v>
+        <v>8665</v>
       </c>
       <c r="F16" s="7">
-        <v>17782280</v>
+        <v>7713</v>
       </c>
       <c r="G16" s="3">
         <v>18000</v>
@@ -1078,6 +3738,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1085,15 +3746,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAFE768-AA87-41D6-9C80-D6513BE5FBC3}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>

</xml_diff>